<commit_message>
Removed 0147 and 0170 again
</commit_message>
<xml_diff>
--- a/publication/v8.1/Peppol Code Lists - Participant identifier schemes v8.1.xlsx
+++ b/publication/v8.1/Peppol Code Lists - Participant identifier schemes v8.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60195E1F-9FFF-4412-B72D-F278515429E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716C22BA-DDD2-4D63-A58D-9CADF896AA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$N$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$N$92</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="526">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -1796,44 +1796,10 @@
     <t>Removal Date</t>
   </si>
   <si>
-    <t>JP:SCC</t>
-  </si>
-  <si>
-    <t>0147</t>
-  </si>
-  <si>
     <t>JP</t>
   </si>
   <si>
-    <t>Standard Company Code</t>
-  </si>
-  <si>
-    <t>JIPDEC</t>
-  </si>
-  <si>
     <t>8.1</t>
-  </si>
-  <si>
-    <t>12 characters (fixed length), First 6 characters identify an organization, Last 6 characters identify an organization part</t>
-  </si>
-  <si>
-    <t>12 characters preceded with 4 digit ICD code</t>
-  </si>
-  <si>
-    <t>JP:TCC</t>
-  </si>
-  <si>
-    <t>0170</t>
-  </si>
-  <si>
-    <t>Teikoku Company Code</t>
-  </si>
-  <si>
-    <t>TEIKOKU DATABANK LTD.</t>
-  </si>
-  <si>
-    <t>1) Eight identification digits and a check digit
-2) One check digit is based on TDB original computation</t>
   </si>
   <si>
     <t>JP:SST</t>
@@ -2706,13 +2672,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMN100"/>
+  <dimension ref="A1:AMN98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G44" sqref="G44"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3199,50 +3165,59 @@
         <v>410</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="240" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>505</v>
+        <v>74</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>506</v>
+        <v>75</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>507</v>
+        <v>76</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>508</v>
+        <v>77</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>509</v>
+        <v>78</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>510</v>
+        <v>79</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>511</v>
+        <v>376</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="240" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>74</v>
+        <v>341</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>75</v>
+        <v>337</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>76</v>
+        <v>214</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>77</v>
+        <v>342</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>78</v>
+        <v>338</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>79</v>
@@ -3251,161 +3226,170 @@
         <v>496</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>376</v>
+        <v>340</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="L15" s="10" t="s">
-        <v>395</v>
+        <v>339</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>513</v>
+        <v>81</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>514</v>
+        <v>82</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>507</v>
+        <v>45</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>515</v>
+        <v>83</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>516</v>
+        <v>83</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>510</v>
+        <v>84</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>517</v>
+        <v>377</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>32</v>
+        <v>385</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="17" spans="1:14 1028:1028" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>341</v>
+        <v>507</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>337</v>
+        <v>508</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>214</v>
+        <v>505</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>342</v>
+        <v>509</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>338</v>
+        <v>510</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>79</v>
+        <v>506</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>340</v>
+        <v>511</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14 1028:1028" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14 1028:1028" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>385</v>
+        <v>386</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>396</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14 1028:1028" ht="150" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14 1028:1028" ht="225" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>518</v>
+        <v>90</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>519</v>
+        <v>91</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>507</v>
+        <v>92</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>520</v>
+        <v>93</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>521</v>
+        <v>94</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>510</v>
+        <v>89</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>522</v>
+        <v>379</v>
       </c>
       <c r="K19" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:14 1028:1028" ht="150" x14ac:dyDescent="0.25">
+      <c r="L19" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14 1028:1028" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>89</v>
@@ -3414,208 +3398,196 @@
         <v>496</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>378</v>
+        <v>100</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>386</v>
+        <v>32</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14 1028:1028" ht="225" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>379</v>
+        <v>107</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L21" s="10" t="s">
-        <v>397</v>
-      </c>
       <c r="M21" s="10" t="s">
-        <v>445</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14 1028:1028" ht="60" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14 1028:1028" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>100</v>
+        <v>380</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L22" s="10" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14 1028:1028" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>107</v>
+        <v>381</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>32</v>
+        <v>388</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14 1028:1028" ht="105" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>108</v>
+        <v>347</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>109</v>
+        <v>345</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>111</v>
+        <v>346</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>112</v>
+        <v>348</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>380</v>
+        <v>349</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>387</v>
+        <v>350</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>448</v>
-      </c>
-      <c r="N24" s="7" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14 1028:1028" ht="105" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14 1028:1028" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>113</v>
+        <v>355</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>114</v>
+        <v>351</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>115</v>
+        <v>35</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>116</v>
+        <v>352</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>117</v>
+        <v>353</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>388</v>
+        <v>354</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14 1028:1028" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>347</v>
+        <v>118</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>345</v>
+        <v>119</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>346</v>
+        <v>121</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>348</v>
+        <v>122</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>79</v>
@@ -3624,205 +3596,208 @@
         <v>496</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>349</v>
+        <v>123</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>350</v>
+        <v>32</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>399</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14 1028:1028" ht="409.5" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14 1028:1028" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="C27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="AMN27" s="7"/>
+    </row>
+    <row r="28" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="AMN28" s="7"/>
+    </row>
+    <row r="29" spans="1:14 1028:1028" ht="165" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="L29" s="12"/>
+      <c r="M29" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="AMN29" s="7"/>
+    </row>
+    <row r="30" spans="1:14 1028:1028" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>382</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>354</v>
-      </c>
-      <c r="M27" s="10" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14 1028:1028" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="K28" s="9" t="s">
+      <c r="D30" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="K30" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L28" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="M28" s="10" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14 1028:1028" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="L30" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="M30" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="AMN30" s="7"/>
+    </row>
+    <row r="31" spans="1:14 1028:1028" ht="255" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>360</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12" t="s">
-        <v>453</v>
-      </c>
-      <c r="N29" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="AMN29" s="7"/>
-    </row>
-    <row r="30" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>360</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>498</v>
-      </c>
-      <c r="K30" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12" t="s">
-        <v>500</v>
-      </c>
-      <c r="N30" s="7" t="s">
-        <v>499</v>
-      </c>
-      <c r="AMN30" s="7"/>
-    </row>
-    <row r="31" spans="1:14 1028:1028" ht="165" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>430</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>425</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="D31" s="7" t="s">
-        <v>426</v>
+        <v>475</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>427</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>428</v>
+        <v>476</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>469</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>465</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>429</v>
+        <v>477</v>
       </c>
       <c r="L31" s="12"/>
       <c r="M31" s="10" t="s">
-        <v>462</v>
+        <v>478</v>
       </c>
       <c r="AMN31" s="7"/>
     </row>
-    <row r="32" spans="1:14 1028:1028" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14 1028:1028" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>467</v>
+        <v>494</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>468</v>
+        <v>479</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>469</v>
@@ -3831,34 +3806,29 @@
         <v>496</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>470</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>472</v>
-      </c>
+        <v>501</v>
+      </c>
+      <c r="L32" s="12"/>
       <c r="M32" s="10" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="AMN32" s="7"/>
     </row>
-    <row r="33" spans="1:14 1028:1028" ht="255" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>475</v>
+        <v>484</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="F33" s="13" t="s">
         <v>469</v>
@@ -3867,29 +3837,32 @@
         <v>496</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>477</v>
+        <v>486</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>487</v>
       </c>
       <c r="L33" s="12"/>
       <c r="M33" s="10" t="s">
-        <v>478</v>
+        <v>488</v>
       </c>
       <c r="AMN33" s="7"/>
     </row>
-    <row r="34" spans="1:14 1028:1028" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>474</v>
+        <v>483</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>479</v>
+        <v>489</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="F34" s="13" t="s">
         <v>469</v>
@@ -3898,171 +3871,167 @@
         <v>496</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>501</v>
+        <v>490</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>491</v>
       </c>
       <c r="L34" s="12"/>
       <c r="M34" s="10" t="s">
-        <v>456</v>
+        <v>492</v>
       </c>
       <c r="AMN34" s="7"/>
     </row>
-    <row r="35" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14 1028:1028" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>480</v>
+        <v>512</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>481</v>
+        <v>513</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>484</v>
+        <v>514</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>485</v>
+        <v>515</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>469</v>
+        <v>506</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>486</v>
+        <v>516</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>487</v>
+        <v>32</v>
       </c>
       <c r="L35" s="12"/>
       <c r="M35" s="10" t="s">
-        <v>488</v>
+        <v>518</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>517</v>
       </c>
       <c r="AMN35" s="7"/>
     </row>
-    <row r="36" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14 1028:1028" ht="240" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>482</v>
+        <v>519</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>483</v>
+        <v>520</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>489</v>
+        <v>521</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>485</v>
+        <v>522</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>469</v>
+        <v>506</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J36" s="9" t="s">
-        <v>490</v>
+        <v>523</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>491</v>
+        <v>32</v>
       </c>
       <c r="L36" s="12"/>
       <c r="M36" s="10" t="s">
-        <v>492</v>
+        <v>525</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>524</v>
       </c>
       <c r="AMN36" s="7"/>
     </row>
-    <row r="37" spans="1:14 1028:1028" ht="150" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14 1028:1028" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>523</v>
+        <v>124</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>524</v>
+        <v>125</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>525</v>
+        <v>126</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>526</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>510</v>
+        <v>126</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="G37" s="17" t="s">
         <v>496</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>527</v>
+        <v>127</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L37" s="12"/>
-      <c r="M37" s="10" t="s">
-        <v>529</v>
-      </c>
       <c r="N37" s="7" t="s">
-        <v>528</v>
-      </c>
-      <c r="AMN37" s="7"/>
-    </row>
-    <row r="38" spans="1:14 1028:1028" ht="240" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>530</v>
+        <v>128</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>531</v>
+        <v>129</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>532</v>
+        <v>130</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>533</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>510</v>
+        <v>130</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>496</v>
       </c>
-      <c r="J38" s="9" t="s">
-        <v>534</v>
-      </c>
-      <c r="K38" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L38" s="12"/>
+      <c r="L38" s="10" t="s">
+        <v>400</v>
+      </c>
       <c r="M38" s="10" t="s">
-        <v>536</v>
-      </c>
-      <c r="N38" s="7" t="s">
-        <v>535</v>
-      </c>
-      <c r="AMN38" s="7"/>
-    </row>
-    <row r="39" spans="1:14 1028:1028" ht="30" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>45</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>13</v>
@@ -4070,31 +4039,28 @@
       <c r="G39" s="17" t="s">
         <v>496</v>
       </c>
-      <c r="J39" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="K39" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="N39" s="7" t="s">
-        <v>415</v>
+      <c r="L39" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="M39" s="10" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="40" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>45</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>13</v>
@@ -4103,117 +4069,126 @@
         <v>496</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="M40" s="10" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14 1028:1028" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>496</v>
+        <v>497</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="J41" s="9" t="s">
+        <v>501</v>
       </c>
       <c r="L41" s="10" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="M41" s="10" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14 1028:1028" ht="285" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>496</v>
+        <v>497</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>506</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>134</v>
+        <v>401</v>
+      </c>
+      <c r="M42" s="10" t="s">
+        <v>457</v>
       </c>
       <c r="N42" s="7" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14 1028:1028" ht="105" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14 1028:1028" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>140</v>
+        <v>147</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>497</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>501</v>
-      </c>
-      <c r="L43" s="10" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="M43" s="10" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14 1028:1028" ht="285" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+      <c r="N43" s="7" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>144</v>
+        <v>344</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>13</v>
@@ -4222,33 +4197,30 @@
         <v>497</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>510</v>
+        <v>150</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>401</v>
+        <v>155</v>
       </c>
       <c r="M44" s="10" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="N44" s="7" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14 1028:1028" ht="60" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14 1028:1028" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>97</v>
+        <v>153</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>13</v>
@@ -4256,32 +4228,24 @@
       <c r="G45" s="17" t="s">
         <v>496</v>
       </c>
-      <c r="J45" s="9" t="s">
-        <v>100</v>
-      </c>
       <c r="M45" s="10" t="s">
-        <v>446</v>
-      </c>
-      <c r="N45" s="7" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14 1028:1028" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>147</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="E46" s="11"/>
       <c r="F46" s="8" t="s">
         <v>13</v>
       </c>
@@ -4291,28 +4255,31 @@
       <c r="H46" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="L46" s="10" t="s">
-        <v>155</v>
+      <c r="J46" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="M46" s="10" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="N46" s="7" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14 1028:1028" ht="90" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14 1028:1028" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>153</v>
+        <v>35</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>154</v>
+        <v>162</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>13</v>
@@ -4320,297 +4287,280 @@
       <c r="G47" s="17" t="s">
         <v>496</v>
       </c>
-      <c r="M47" s="10" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14 1028:1028" ht="75" x14ac:dyDescent="0.25">
+      <c r="N47" s="7" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14 1028:1028" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E48" s="11"/>
+        <v>166</v>
+      </c>
       <c r="F48" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>497</v>
-      </c>
-      <c r="H48" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="J48" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="M48" s="10" t="s">
-        <v>460</v>
-      </c>
-      <c r="N48" s="7" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+        <v>496</v>
+      </c>
+      <c r="L48" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>162</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="E49" s="11"/>
       <c r="F49" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>496</v>
       </c>
+      <c r="L49" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="M49" s="10" t="s">
+        <v>461</v>
+      </c>
       <c r="N49" s="7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>165</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="L50" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>497</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E51" s="11"/>
+        <v>117</v>
+      </c>
       <c r="F51" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G51" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="L51" s="10" t="s">
-        <v>402</v>
+        <v>497</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J51" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="K51" s="9" t="s">
+        <v>388</v>
       </c>
       <c r="M51" s="10" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="N51" s="7" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="C52" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="J52" s="9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G52" s="17" t="s">
+      <c r="D53" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E53" s="11"/>
+      <c r="F53" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="J53" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="N53" s="7" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G55" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="H52" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" ht="105" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>497</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J53" s="9" t="s">
-        <v>381</v>
-      </c>
-      <c r="K53" s="9" t="s">
-        <v>388</v>
-      </c>
-      <c r="M53" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="N53" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="G54" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="J54" s="9" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="E55" s="11"/>
-      <c r="F55" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="G55" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="J55" s="9" t="s">
-        <v>187</v>
+      <c r="H55" s="8" t="s">
+        <v>360</v>
       </c>
       <c r="N55" s="7" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>188</v>
+        <v>423</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>193</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>175</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="E56" s="11"/>
       <c r="F56" s="8" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="G56" s="17" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>191</v>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>197</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>51</v>
+        <v>199</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>179</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="E57" s="11"/>
       <c r="F57" s="8" t="s">
         <v>150</v>
       </c>
       <c r="G57" s="17" t="s">
-        <v>497</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>360</v>
-      </c>
-      <c r="N57" s="7" t="s">
-        <v>423</v>
+        <v>496</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="E58" s="11"/>
       <c r="F58" s="8" t="s">
@@ -4622,16 +4572,16 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>199</v>
+        <v>103</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E59" s="11"/>
       <c r="F59" s="8" t="s">
@@ -4643,16 +4593,16 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="E60" s="11"/>
       <c r="F60" s="8" t="s">
@@ -4664,16 +4614,16 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>103</v>
+        <v>214</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="E61" s="11"/>
       <c r="F61" s="8" t="s">
@@ -4685,18 +4635,17 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="E62" s="11"/>
+        <v>219</v>
+      </c>
       <c r="F62" s="8" t="s">
         <v>150</v>
       </c>
@@ -4706,16 +4655,16 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E63" s="11"/>
       <c r="F63" s="8" t="s">
@@ -4727,17 +4676,18 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>219</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="E64" s="11"/>
       <c r="F64" s="8" t="s">
         <v>150</v>
       </c>
@@ -4747,16 +4697,16 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>222</v>
+        <v>92</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="E65" s="11"/>
       <c r="F65" s="8" t="s">
@@ -4767,17 +4717,17 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="14" t="s">
-        <v>224</v>
+      <c r="A66" s="15" t="s">
+        <v>231</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="E66" s="11"/>
       <c r="F66" s="8" t="s">
@@ -4788,17 +4738,17 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
-        <v>228</v>
+      <c r="A67" s="15" t="s">
+        <v>235</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>92</v>
+        <v>237</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="E67" s="11"/>
       <c r="F67" s="8" t="s">
@@ -4810,16 +4760,16 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="E68" s="11"/>
       <c r="F68" s="8" t="s">
@@ -4831,16 +4781,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="E69" s="11"/>
       <c r="F69" s="8" t="s">
@@ -4852,16 +4802,16 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="E70" s="11"/>
       <c r="F70" s="8" t="s">
@@ -4873,16 +4823,16 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>245</v>
+        <v>120</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="E71" s="11"/>
       <c r="F71" s="8" t="s">
@@ -4894,16 +4844,16 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="E72" s="11"/>
       <c r="F72" s="8" t="s">
@@ -4915,16 +4865,16 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="E73" s="11"/>
       <c r="F73" s="8" t="s">
@@ -4936,16 +4886,16 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="E74" s="11"/>
       <c r="F74" s="8" t="s">
@@ -4957,16 +4907,16 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E75" s="11"/>
       <c r="F75" s="8" t="s">
@@ -4976,18 +4926,18 @@
         <v>496</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E76" s="11"/>
       <c r="F76" s="8" t="s">
@@ -4999,16 +4949,16 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="E77" s="11"/>
       <c r="F77" s="8" t="s">
@@ -5018,18 +4968,18 @@
         <v>496</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>272</v>
+        <v>55</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="E78" s="11"/>
       <c r="F78" s="8" t="s">
@@ -5041,16 +4991,16 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="E79" s="11"/>
       <c r="F79" s="8" t="s">
@@ -5062,16 +5012,16 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>55</v>
+        <v>287</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="E80" s="11"/>
       <c r="F80" s="8" t="s">
@@ -5083,16 +5033,16 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="E81" s="11"/>
       <c r="F81" s="8" t="s">
@@ -5101,19 +5051,20 @@
       <c r="G81" s="17" t="s">
         <v>496</v>
       </c>
+      <c r="I81" s="3"/>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="E82" s="11"/>
       <c r="F82" s="8" t="s">
@@ -5122,19 +5073,20 @@
       <c r="G82" s="17" t="s">
         <v>496</v>
       </c>
+      <c r="I82" s="3"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="E83" s="11"/>
       <c r="F83" s="8" t="s">
@@ -5147,16 +5099,16 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="E84" s="11"/>
       <c r="F84" s="8" t="s">
@@ -5165,42 +5117,39 @@
       <c r="G84" s="17" t="s">
         <v>496</v>
       </c>
-      <c r="I84" s="3"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="E85" s="11"/>
+        <v>308</v>
+      </c>
       <c r="F85" s="8" t="s">
         <v>150</v>
       </c>
       <c r="G85" s="17" t="s">
         <v>496</v>
       </c>
-      <c r="I85" s="3"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="E86" s="11"/>
       <c r="F86" s="8" t="s">
@@ -5209,20 +5158,22 @@
       <c r="G86" s="17" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I86" s="4"/>
+    </row>
+    <row r="87" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>308</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="E87" s="11"/>
       <c r="F87" s="8" t="s">
         <v>150</v>
       </c>
@@ -5231,184 +5182,141 @@
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A88" s="15" t="s">
-        <v>309</v>
+      <c r="A88" s="7" t="s">
+        <v>317</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>311</v>
+        <v>55</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="E88" s="11"/>
+        <v>319</v>
+      </c>
       <c r="F88" s="8" t="s">
-        <v>150</v>
+        <v>320</v>
       </c>
       <c r="G88" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="I88" s="4"/>
-    </row>
-    <row r="89" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="15" t="s">
-        <v>313</v>
+        <v>497</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I88" s="3"/>
+      <c r="N88" s="7" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A89" s="7" t="s">
+        <v>322</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>315</v>
+        <v>17</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="E89" s="11"/>
+        <v>324</v>
+      </c>
       <c r="F89" s="8" t="s">
-        <v>150</v>
+        <v>325</v>
       </c>
       <c r="G89" s="17" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I89" s="3"/>
+    </row>
+    <row r="90" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>319</v>
+        <v>328</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>329</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>320</v>
+        <v>84</v>
       </c>
       <c r="G90" s="17" t="s">
         <v>497</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>89</v>
+        <v>464</v>
       </c>
       <c r="I90" s="3"/>
-      <c r="N90" s="7" t="s">
-        <v>321</v>
+      <c r="J90" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="L90" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="M90" s="10" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>325</v>
+        <v>84</v>
       </c>
       <c r="G91" s="17" t="s">
         <v>496</v>
       </c>
-      <c r="I91" s="3"/>
-    </row>
-    <row r="92" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>103</v>
+        <v>226</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="G92" s="17" t="s">
         <v>497</v>
       </c>
       <c r="H92" s="8" t="s">
-        <v>464</v>
-      </c>
-      <c r="I92" s="3"/>
-      <c r="J92" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="L92" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="M92" s="10" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A93" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="F93" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G93" s="17" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A94" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="F94" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G94" s="17" t="s">
-        <v>497</v>
-      </c>
-      <c r="H94" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="I94" s="4"/>
-      <c r="N94" s="7" t="s">
+      <c r="I92" s="4"/>
+      <c r="N92" s="7" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I100" s="4"/>
+    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I98" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N94" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:N92" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>

</xml_diff>